<commit_message>
cek datahli waris, failed. back to basic
</commit_message>
<xml_diff>
--- a/sert example.xlsx
+++ b/sert example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\#Data Kabir\deep analysis\wp full analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14A007E5-2FC6-4E29-8804-772C64C8ACF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B4E572-3CEE-4CD9-A8DC-DBE82D8D97B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="55">
   <si>
     <t>Nama</t>
   </si>
@@ -128,6 +128,66 @@
   </si>
   <si>
     <t>wa harna, la amin, wa ulfa</t>
+  </si>
+  <si>
+    <t>HUSNAWATI,S.PD.-</t>
+  </si>
+  <si>
+    <t>00632</t>
+  </si>
+  <si>
+    <t>HJ. SITTI HARIANA, S.ST,KER</t>
+  </si>
+  <si>
+    <t>00095</t>
+  </si>
+  <si>
+    <t>SUJALIL, ST</t>
+  </si>
+  <si>
+    <t>00145</t>
+  </si>
+  <si>
+    <t>LA FAIDI, SP</t>
+  </si>
+  <si>
+    <t>00144</t>
+  </si>
+  <si>
+    <t>IDHAM KASMIN, SE</t>
+  </si>
+  <si>
+    <t>00257</t>
+  </si>
+  <si>
+    <t>IKHVAN KASMIN, SH</t>
+  </si>
+  <si>
+    <t>00259</t>
+  </si>
+  <si>
+    <t>TUTI ALAMIA, S. PD SD</t>
+  </si>
+  <si>
+    <t>00260</t>
+  </si>
+  <si>
+    <t>ARDIN, SE</t>
+  </si>
+  <si>
+    <t>00379</t>
+  </si>
+  <si>
+    <t>TARFAN, S. PD</t>
+  </si>
+  <si>
+    <t>00316</t>
+  </si>
+  <si>
+    <t>00398</t>
+  </si>
+  <si>
+    <t>00317</t>
   </si>
 </sst>
 </file>
@@ -210,7 +270,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -218,7 +278,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -534,10 +593,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="A33" sqref="A33:C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -774,14 +833,146 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B21">
         <v>12345</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C21" s="2">
         <v>2000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23">
+        <v>9207</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24">
+        <v>4237</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25">
+        <v>6480</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26">
+        <v>9665</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>45</v>
+      </c>
+      <c r="B27" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27">
+        <v>9665</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>47</v>
+      </c>
+      <c r="B28" t="s">
+        <v>48</v>
+      </c>
+      <c r="C28">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>49</v>
+      </c>
+      <c r="B29" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>51</v>
+      </c>
+      <c r="B30" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30">
+        <v>11790</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>51</v>
+      </c>
+      <c r="B31" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>51</v>
+      </c>
+      <c r="B32" t="s">
+        <v>54</v>
+      </c>
+      <c r="C32">
+        <v>12310</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" s="2">
+        <v>20000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>